<commit_message>
paper edited: total number of features list corrected in table 2
</commit_message>
<xml_diff>
--- a/Dataset/feature importance/feature_selection.xlsx
+++ b/Dataset/feature importance/feature_selection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Works\NSU\CSE419\repository\CSE419-Sensor-Data-based-Activity-Classification\Dataset\feature importance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1D0FBB-F3EC-44C6-B2E3-1181CD117BBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5ED91ED-7B38-4AEC-A01F-F3684B562918}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="825" yWindow="-120" windowWidth="19785" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="121">
   <si>
     <t>lastSensorEventHours</t>
   </si>
@@ -385,6 +385,9 @@
   </si>
   <si>
     <t>Random forest classifer</t>
+  </si>
+  <si>
+    <t>Total Feature Set</t>
   </si>
 </sst>
 </file>
@@ -837,10 +840,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AL51"/>
+  <dimension ref="A1:AL52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1794,6 +1797,9 @@
       <c r="E15" s="19" t="s">
         <v>119</v>
       </c>
+      <c r="J15" s="10" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="16" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
@@ -1808,8 +1814,11 @@
       <c r="E16" s="20" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J16" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>37</v>
       </c>
@@ -1822,8 +1831,11 @@
       <c r="E17" s="20" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>38</v>
       </c>
@@ -1834,8 +1846,11 @@
       <c r="E18" s="20" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="18"/>
       <c r="B19" s="10" t="s">
         <v>74</v>
@@ -1846,8 +1861,11 @@
       <c r="E19" s="20" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="17"/>
       <c r="B20" s="17"/>
       <c r="D20" s="20" t="s">
@@ -1856,8 +1874,11 @@
       <c r="E20" s="20" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>5</v>
       </c>
@@ -1868,8 +1889,11 @@
       <c r="E21" s="20" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="17"/>
       <c r="B22" s="17"/>
       <c r="D22" s="20" t="s">
@@ -1878,8 +1902,11 @@
       <c r="E22" s="20" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="17"/>
       <c r="B23" s="17"/>
       <c r="D23" s="20" t="s">
@@ -1888,8 +1915,11 @@
       <c r="E23" s="20" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>42</v>
       </c>
@@ -1900,8 +1930,11 @@
       <c r="E24" s="20" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>62</v>
       </c>
@@ -1914,8 +1947,11 @@
       <c r="E25" s="20" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="17"/>
       <c r="B26" s="17"/>
       <c r="D26" s="20" t="s">
@@ -1924,8 +1960,11 @@
       <c r="E26" s="20" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="17"/>
       <c r="B27" s="17"/>
       <c r="D27" s="20" t="s">
@@ -1934,8 +1973,11 @@
       <c r="E27" s="20" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="17"/>
       <c r="B28" s="17"/>
       <c r="D28" s="20" t="s">
@@ -1944,8 +1986,11 @@
       <c r="E28" s="20" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="17"/>
       <c r="B29" s="17"/>
       <c r="D29" s="20" t="s">
@@ -1954,8 +1999,11 @@
       <c r="E29" s="20" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="18"/>
       <c r="B30" s="17"/>
       <c r="D30" s="20" t="s">
@@ -1964,8 +2012,11 @@
       <c r="E30" s="20" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="17"/>
       <c r="B31" s="17"/>
       <c r="D31" s="20" t="s">
@@ -1974,8 +2025,11 @@
       <c r="E31" s="20" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="17"/>
       <c r="B32" s="17"/>
       <c r="D32" s="20" t="s">
@@ -1984,8 +2038,11 @@
       <c r="E32" s="20" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="17"/>
       <c r="B33" s="17"/>
       <c r="D33" s="20" t="s">
@@ -1994,8 +2051,11 @@
       <c r="E33" s="20" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J33" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="17"/>
       <c r="B34" s="17"/>
       <c r="D34" s="20" t="s">
@@ -2004,8 +2064,11 @@
       <c r="E34" s="20" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J34" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="17"/>
       <c r="B35" s="17"/>
       <c r="D35" s="20" t="s">
@@ -2014,8 +2077,11 @@
       <c r="E35" s="20" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J35" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>10</v>
       </c>
@@ -2028,86 +2094,139 @@
       <c r="E36" s="20" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J36" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="17"/>
       <c r="B38" s="10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J38" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="17"/>
       <c r="B39" s="17"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J39" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="17"/>
       <c r="B40" s="17"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J40" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B41" s="10" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J41" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="17"/>
       <c r="B42" s="17"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J42" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
         <v>51</v>
       </c>
       <c r="B43" s="10" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J44" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="18"/>
       <c r="B45" s="18"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J45" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="18"/>
       <c r="B46" s="18"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J46" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
         <v>54</v>
       </c>
       <c r="B47" s="10" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J47" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="17"/>
       <c r="B48" s="17"/>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J48" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="18"/>
       <c r="B49" s="18"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J49" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B50" s="10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J50" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
         <v>56</v>
+      </c>
+      <c r="J51" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J52" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>